<commit_message>
Code update, schematic plots, text update
</commit_message>
<xml_diff>
--- a/docs/bom/GPS-Compass_GNSS_BOM.xlsx
+++ b/docs/bom/GPS-Compass_GNSS_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\GPS-Compass\docs\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D98BA4E-EF7A-41C7-8D74-C0FA7EFA54EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1AE8B2-1DFA-4530-B479-1595576EB5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="900" windowWidth="29040" windowHeight="15720" xr2:uid="{318D0819-0F8D-4535-926A-50240C04F6C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{318D0819-0F8D-4535-926A-50240C04F6C9}"/>
   </bookViews>
   <sheets>
     <sheet name="GPS-Compass_main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>Value</t>
   </si>
@@ -89,18 +89,12 @@
     <t>U1</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>AE1</t>
   </si>
   <si>
     <t>Antenna</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Quectel/YCGO005AA?qs=7D1LtPJG0i2jU0GyBGV%252BDQ%3D%3D</t>
-  </si>
-  <si>
     <t>C1,C3</t>
   </si>
   <si>
@@ -113,33 +107,21 @@
     <t>1n</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Murata-Electronics/GRM1555C2A102JE01J?qs=d0WKAl%252BL4KaQ0kf9CfZNPg%3D%3D</t>
-  </si>
-  <si>
     <t>C4,C6</t>
   </si>
   <si>
     <t>56n</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Murata-Electronics/GRM155R71C563JA88D?qs=IPQhFcwEUOhUUKpBBiLlZQ%3D%3D</t>
-  </si>
-  <si>
     <t>C5,C8</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Murata-Electronics/GRM21BR71C475KE51K?qs=GtmDRopnxzr%2F5bkS0ZUcHw%3D%3D,https://cz.mouser.com/ProductDetail/TDK/CGA2B3X7R1H103K050BE?qs=nQSIdc08i%252BdRFt1oFHRWEA%3D%3D</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
     <t>10n</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/TDK/CGA2B3X7R1H103K050BE?qs=nQSIdc08i%252BdRFt1oFHRWEA%3D%3D</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -158,9 +140,6 @@
     <t>B39162B4327P810</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/RF360/B39162B4327P810?qs=lGUynpphgXxwtn5A8O%2FIyg%3D%3D</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -170,9 +149,6 @@
     <t>gps-compass_brd:636101112001</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Wurth-Elektronik/636101112001?qs=iLbezkQI%252BshOHZpPZv%252BznA%3D%3D&amp;mgh=1&amp;utm_id=20233080446&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_marketing_tactic=emeacorp&amp;gad_source=1&amp;gad_campaignid=20233099895&amp;gclid=CjwKCAiAlMHIBhAcEiwAZhZBUqJNehQU9m-ma0pKSysxiRcQ371froHoDfgmOxQXZoqrNxiS6vIbvxoCynMQAvD_BwE</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -182,24 +158,15 @@
     <t>Inductor_SMD:L_0402_1005Metric</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/TDK/MLG1005S5N6ST000?qs=BanKw8U3RZanzbQ3uYkDLw%3D%3D</t>
-  </si>
-  <si>
     <t>27nH</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Murata-Electronics/LQG15HS27NJ02D?qs=ctz47l0uL1AbPpSO0oLF1A%3D%3D</t>
-  </si>
-  <si>
     <t>MMBT3904</t>
   </si>
   <si>
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Diotec-Semiconductor/MMBT3904?qs=OlC7AqGiEDkK1MwiyUU6mg%3D%3D</t>
-  </si>
-  <si>
     <t>R1,R2,R3</t>
   </si>
   <si>
@@ -230,16 +197,7 @@
     <t>BGA725L6E6327FTSA1</t>
   </si>
   <si>
-    <t>https://cz.mouser.com/ProductDetail/Infineon-Technologies/BGA725L6E6327FTSA1?qs=4MqXaUMeF57lT69yR2PUGQ%3D%3D</t>
-  </si>
-  <si>
     <t>TESEO-LIV3R</t>
-  </si>
-  <si>
-    <t>https://cz.mouser.com/ProductDetail/STMicroelectronics/TESEO-LIV3R?qs=sGAEpiMZZMu3sxpa5v1qrvImzcqkHJqszJjyNiOPDaE%3D</t>
-  </si>
-  <si>
-    <t>https://cz.mouser.com/ProductDetail/Murata-Electronics/GCM1555C2A121JE02D?qs=ZcfC38r4Posmjmarb1xIkw%3D%3</t>
   </si>
   <si>
     <t>120pF, 100V, 0402, ceramic</t>
@@ -1274,10 +1232,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C378E24-255E-4758-9EA3-ADC3BD7350B6}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="H2:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,84 +1278,76 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>21</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>68</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>26</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>29</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1408,33 +1361,29 @@
       <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
+      <c r="H6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>34</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1443,13 +1392,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1458,39 +1407,35 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
+      <c r="H9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>41</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1505,57 +1450,55 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="H12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H14"/>
     </row>
@@ -1564,47 +1507,43 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" t="s">
-        <v>49</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="H15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>51</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1613,18 +1552,16 @@
         <v>7</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>54</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1633,65 +1570,61 @@
         <v>7</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>65</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>67</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2026,33 +1959,23 @@
     <sortCondition ref="B2:B21"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{2C19EA54-5D33-456A-842F-BD08470A48B9}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{41F4D6FD-AC8F-48C8-8139-FD05564F028D}"/>
-    <hyperlink ref="F3" r:id="rId3" display="120pF, 100V, 0402" xr:uid="{F715C98D-9270-4384-8945-C412861EA6FB}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{AE93A21E-596B-41EA-BACB-0DEAAF5EDE64}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{743DEBF8-50A9-4C79-AC49-2EB97AF676D5}"/>
-    <hyperlink ref="H5" r:id="rId6" xr:uid="{4061A4DD-3D3B-4F15-B703-125D982CD595}"/>
-    <hyperlink ref="F5" r:id="rId7" xr:uid="{B6675CEB-E110-47C5-82B4-72E5EF5CEC98}"/>
-    <hyperlink ref="F6" r:id="rId8" display="100nF, 16V, 0805, ceramic, mouser X7R" xr:uid="{210F146F-B18D-4C98-A96F-34A3DECA80E9}"/>
-    <hyperlink ref="H7" r:id="rId9" xr:uid="{9767A593-D0DE-4F35-8D65-DCAE218D9C22}"/>
-    <hyperlink ref="F7" r:id="rId10" xr:uid="{C18D6396-CC99-467C-8499-373B782ED860}"/>
-    <hyperlink ref="H13" r:id="rId11" display="https://cz.mouser.com/ProductDetail/Wurth-Elektronik/636101112001?qs=iLbezkQI%252BshOHZpPZv%252BznA%3D%3D&amp;mgh=1&amp;utm_id=20233080446&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_marketing_tactic=emeacorp&amp;gad_source=1&amp;gad_campaignid=20233099895&amp;gclid=CjwKCAiAlMHIBhAcEiwAZhZBUqJNehQU9m-ma0pKSysxiRcQ371froHoDfgmOxQXZoqrNxiS6vIbvxoCynMQAvD_BwE" xr:uid="{BD223F35-1A02-4A2E-9A07-160D6A3974EF}"/>
-    <hyperlink ref="F12" r:id="rId12" xr:uid="{475477C9-0C06-4FCB-9CF3-E6684D7BEA6E}"/>
-    <hyperlink ref="H10" r:id="rId13" xr:uid="{8D67FE6D-C793-4583-85CB-C47528B5F9AD}"/>
-    <hyperlink ref="F10" r:id="rId14" xr:uid="{C5FD29A9-F38E-4922-AE73-E2A4A874D8EF}"/>
-    <hyperlink ref="H19" r:id="rId15" xr:uid="{052F874A-78CE-472B-9EF3-E1A319720C2A}"/>
-    <hyperlink ref="H20" r:id="rId16" xr:uid="{047BB56D-0C87-4549-9C36-B96522905106}"/>
-    <hyperlink ref="H16" r:id="rId17" xr:uid="{436FDA2D-A1E1-4AD5-A365-5F2ABC0908DD}"/>
-    <hyperlink ref="F14" r:id="rId18" xr:uid="{EEA5DBF6-81EF-47E1-8FAD-E0471AE971CE}"/>
-    <hyperlink ref="F13" r:id="rId19" xr:uid="{FD5DA6F0-EE08-459D-8615-1D1C02A7DF2C}"/>
-    <hyperlink ref="F15" r:id="rId20" xr:uid="{B6BF4F6B-EE73-41DA-B818-4F96BCA51226}"/>
-    <hyperlink ref="H17" r:id="rId21" xr:uid="{B6A3AA18-9CC3-4517-9C9B-1EA3EEE1C9D9}"/>
-    <hyperlink ref="F21" r:id="rId22" xr:uid="{A35F6518-A084-49D2-885A-D412E0FD7621}"/>
-    <hyperlink ref="F17" r:id="rId23" xr:uid="{BF5B4FF6-A686-4182-B171-C7051A270B24}"/>
-    <hyperlink ref="F16" r:id="rId24" xr:uid="{81917A0D-9A80-4A2E-951A-721C0DD80994}"/>
-    <hyperlink ref="F2" r:id="rId25" xr:uid="{31B62545-CCD0-449A-B343-372BEB300B3F}"/>
-    <hyperlink ref="F20" r:id="rId26" xr:uid="{CCB2A479-31CD-492F-88A1-3166C6435F3A}"/>
+    <hyperlink ref="F3" r:id="rId1" display="120pF, 100V, 0402" xr:uid="{F715C98D-9270-4384-8945-C412861EA6FB}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{743DEBF8-50A9-4C79-AC49-2EB97AF676D5}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{B6675CEB-E110-47C5-82B4-72E5EF5CEC98}"/>
+    <hyperlink ref="F6" r:id="rId4" display="100nF, 16V, 0805, ceramic, mouser X7R" xr:uid="{210F146F-B18D-4C98-A96F-34A3DECA80E9}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{C18D6396-CC99-467C-8499-373B782ED860}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{475477C9-0C06-4FCB-9CF3-E6684D7BEA6E}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{C5FD29A9-F38E-4922-AE73-E2A4A874D8EF}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{EEA5DBF6-81EF-47E1-8FAD-E0471AE971CE}"/>
+    <hyperlink ref="F13" r:id="rId9" xr:uid="{FD5DA6F0-EE08-459D-8615-1D1C02A7DF2C}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{B6BF4F6B-EE73-41DA-B818-4F96BCA51226}"/>
+    <hyperlink ref="F21" r:id="rId11" xr:uid="{A35F6518-A084-49D2-885A-D412E0FD7621}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{BF5B4FF6-A686-4182-B171-C7051A270B24}"/>
+    <hyperlink ref="F16" r:id="rId13" xr:uid="{81917A0D-9A80-4A2E-951A-721C0DD80994}"/>
+    <hyperlink ref="F2" r:id="rId14" xr:uid="{31B62545-CCD0-449A-B343-372BEB300B3F}"/>
+    <hyperlink ref="F20" r:id="rId15" xr:uid="{CCB2A479-31CD-492F-88A1-3166C6435F3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="24" orientation="landscape" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>